<commit_message>
Extra tickets + overzicht bijwerkt
</commit_message>
<xml_diff>
--- a/overzicht.xlsx
+++ b/overzicht.xlsx
@@ -465,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -490,12 +490,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -509,12 +503,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -828,7 +816,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -839,8 +827,8 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,274 +862,274 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="16" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="13" t="s">
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="13" t="s">
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="13" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="13" t="s">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="14" t="s">
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="13" t="s">
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="11" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="13" t="s">
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="13" t="s">
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="11" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="13" t="s">
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="16" t="s">
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="16" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="13" t="s">
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="13" t="s">
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="11" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="13" t="s">
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="29" t="s">
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="13" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="13" t="s">
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="11" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="13" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="11" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="31"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="16" t="s">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="29" t="s">
+      <c r="D22" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="30"/>
-      <c r="F22" s="15" t="s">
+      <c r="E22" s="26"/>
+      <c r="F22" s="13" t="s">
         <v>37</v>
       </c>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="13" t="s">
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="11" t="s">
         <v>38</v>
       </c>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="14" t="s">
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="12" t="s">
         <v>39</v>
       </c>
       <c r="G24" s="3"/>
@@ -1156,50 +1144,50 @@
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="10" t="s">
         <v>41</v>
       </c>
       <c r="E26" s="8"/>
-      <c r="F26" s="19" t="s">
+      <c r="F26" s="15" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="29" t="s">
+      <c r="D27" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="29" t="s">
+      <c r="E27" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="F27" s="16" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="31"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="14" t="s">
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="12" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1213,42 +1201,42 @@
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="30" t="s">
+      <c r="D30" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="E30" s="28" t="s">
+      <c r="E30" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="F30" s="13" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="13" t="s">
+      <c r="A31" s="26"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="11" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="31"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="14" t="s">
+      <c r="A32" s="27"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="12" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1265,48 +1253,48 @@
       <c r="D33" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="27"/>
-      <c r="F33" s="21" t="s">
+      <c r="E33" s="23"/>
+      <c r="F33" s="17" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="28" t="s">
+      <c r="C34" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="D34" s="28" t="s">
+      <c r="D34" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="E34" s="28" t="s">
+      <c r="E34" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="F34" s="22" t="s">
+      <c r="F34" s="18" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="23" t="s">
+      <c r="A35" s="22"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="19" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="27"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="24" t="s">
+      <c r="A36" s="23"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="20" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1320,170 +1308,137 @@
       <c r="G37" s="7"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="28" t="s">
+      <c r="A38" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="B38" s="28" t="s">
+      <c r="B38" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="28" t="s">
+      <c r="C38" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="E38" s="28" t="s">
+      <c r="E38" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F38" s="13" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="27"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="10" t="s">
+      <c r="A39" s="23"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="12" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="25" t="s">
+      <c r="A40" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="B40" s="25" t="s">
+      <c r="B40" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="25" t="s">
+      <c r="C40" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D40" s="25" t="s">
+      <c r="D40" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="E40" s="25" t="s">
+      <c r="E40" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="F40" s="18" t="s">
+      <c r="F40" s="16" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="26"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="17" t="s">
+      <c r="A41" s="22"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="11" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="17" t="s">
+      <c r="A42" s="22"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="11" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="17" t="s">
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="11" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="17" t="s">
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="11" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="17" t="s">
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="11" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="17" t="s">
+      <c r="A46" s="22"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="11" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="26"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="17" t="s">
+      <c r="A47" s="22"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="11" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="27"/>
-      <c r="B48" s="27"/>
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="16" t="s">
+      <c r="A48" s="23"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="23"/>
+      <c r="F48" s="12" t="s">
         <v>74</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="A14:A21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="B14:B21"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="E40:E48"/>
-    <mergeCell ref="D40:D48"/>
-    <mergeCell ref="C40:C48"/>
-    <mergeCell ref="B40:B48"/>
-    <mergeCell ref="A40:A48"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C34:C36"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
     <mergeCell ref="E2:E7"/>
     <mergeCell ref="E8:E13"/>
     <mergeCell ref="E14:E17"/>
@@ -1496,6 +1451,39 @@
     <mergeCell ref="D8:D13"/>
     <mergeCell ref="D14:D21"/>
     <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:C36"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="E40:E48"/>
+    <mergeCell ref="D40:D48"/>
+    <mergeCell ref="C40:C48"/>
+    <mergeCell ref="B40:B48"/>
+    <mergeCell ref="A40:A48"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A14:A21"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="B14:B21"/>
+    <mergeCell ref="B22:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1503,6 +1491,29 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <jeb5123c558143d5ab1e1526e87a8da0 xmlns="b7e4e9fd-5e36-4299-889f-f6136aff670e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </jeb5123c558143d5ab1e1526e87a8da0>
+    <Cohort xmlns="b7e4e9fd-5e36-4299-889f-f6136aff670e"/>
+    <TaxCatchAll xmlns="fbafb59e-d651-4668-8e65-f7f85ceca18b"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C5151218AB56640BDBA68249A073511" ma:contentTypeVersion="23" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="a1da3f48426d5c2cead333d31125cb2a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="b7e4e9fd-5e36-4299-889f-f6136aff670e" xmlns:ns3="fbafb59e-d651-4668-8e65-f7f85ceca18b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1529523bac735da72c0db022ce5932da" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1777,45 +1788,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <jeb5123c558143d5ab1e1526e87a8da0 xmlns="b7e4e9fd-5e36-4299-889f-f6136aff670e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </jeb5123c558143d5ab1e1526e87a8da0>
-    <Cohort xmlns="b7e4e9fd-5e36-4299-889f-f6136aff670e"/>
-    <TaxCatchAll xmlns="fbafb59e-d651-4668-8e65-f7f85ceca18b"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A1289EE-009B-46B8-AE36-FD2598B812B5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE469190-2D20-42A2-9E3F-DFC4A4FB0F31}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="b7e4e9fd-5e36-4299-889f-f6136aff670e"/>
-    <ds:schemaRef ds:uri="fbafb59e-d651-4668-8e65-f7f85ceca18b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1839,9 +1815,21 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE469190-2D20-42A2-9E3F-DFC4A4FB0F31}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A1289EE-009B-46B8-AE36-FD2598B812B5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="b7e4e9fd-5e36-4299-889f-f6136aff670e"/>
+    <ds:schemaRef ds:uri="fbafb59e-d651-4668-8e65-f7f85ceca18b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>